<commit_message>
Milestone 3 Turn in
To be graded updated rubric included
</commit_message>
<xml_diff>
--- a/GraphicsProject/Boza.Jason.Graphics II Project Rubric.xlsx
+++ b/GraphicsProject/Boza.Jason.Graphics II Project Rubric.xlsx
@@ -94,6 +94,31 @@
           </rPr>
           <t xml:space="preserve">
 Ocean</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+1 = default rasterstate
+2 = wireframe</t>
         </r>
       </text>
     </comment>
@@ -202,7 +227,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="87">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -1035,8 +1060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1172,15 +1197,15 @@
       </c>
       <c r="J4" s="5">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="K4" s="5">
         <f>SUM(H6,I6,J6)</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>50</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1253,12 +1278,12 @@
       </c>
       <c r="J6" s="5">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 22, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) - 22,0)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="9">
         <f>IF(L4 &gt; 66, SUM(-66,L4),0)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1305,11 +1330,15 @@
       <c r="D8" s="5">
         <v>5</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
+      <c r="E8" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G8" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H8" s="10">
         <f>H4+IF(H4 &lt; 22, IF(K4+H4 &gt; 22, 22- H4, K4),0)</f>
@@ -1321,7 +1350,7 @@
       </c>
       <c r="J8" s="9">
         <f>J4+IF(J4 &lt; 22, IF(I10+J4 &gt; 22, 22- J4, I10),0)</f>
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1378,15 +1407,15 @@
       </c>
       <c r="H10" s="5">
         <f>IF(K4+H4 - 22 &gt; 0, K4+H4 - 22, 0)</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I10" s="5">
         <f>IF(H10+I4 - 22 &gt; 0, H10+I4 - 22, 0)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J10" s="5">
         <f>IF(I10+J4 - 22 &gt; 0, I10+J4 - 22, 0)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -1832,11 +1861,15 @@
       <c r="D31" s="5">
         <v>3</v>
       </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="3"/>
+      <c r="E31" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G31" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
@@ -1857,11 +1890,15 @@
       <c r="D32" s="5">
         <v>3</v>
       </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="3"/>
+      <c r="E32" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G32" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
@@ -1882,11 +1919,15 @@
       <c r="D33" s="5">
         <v>1</v>
       </c>
-      <c r="E33" s="2"/>
-      <c r="F33" s="3"/>
+      <c r="E33" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G33" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
@@ -1907,11 +1948,15 @@
       <c r="D34" s="5">
         <v>1</v>
       </c>
-      <c r="E34" s="2"/>
-      <c r="F34" s="3"/>
+      <c r="E34" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G34" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
@@ -1932,11 +1977,15 @@
       <c r="D35" s="5">
         <v>1</v>
       </c>
-      <c r="E35" s="2"/>
-      <c r="F35" s="3"/>
+      <c r="E35" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G35" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
@@ -1957,11 +2006,15 @@
       <c r="D36" s="5">
         <v>2</v>
       </c>
-      <c r="E36" s="2"/>
-      <c r="F36" s="3"/>
+      <c r="E36" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G36" s="8">
         <f t="shared" ref="G36:G67" si="1" xml:space="preserve"> IF(EXACT(F36,"X"),IF(EXACT(E36,"I"),$B36,IF(EXACT(E36,"II"),$C36,IF(EXACT(E36,"III"),$D36,0))),0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
@@ -2339,11 +2392,15 @@
       <c r="D54" s="5">
         <v>3</v>
       </c>
-      <c r="E54" s="2"/>
-      <c r="F54" s="3"/>
+      <c r="E54" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G54" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
@@ -3033,7 +3090,9 @@
       <c r="D90" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E90" s="3"/>
+      <c r="E90" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="F90" s="5"/>
       <c r="G90" s="5"/>
       <c r="H90" s="5"/>
@@ -3202,7 +3261,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>